<commit_message>
tshirt_inventory_redacted: Add data validation.
Ignore UserWarnings in the scripts (openpyxl does not support them).
</commit_message>
<xml_diff>
--- a/tshirt_inventory_redacted.xlsx
+++ b/tshirt_inventory_redacted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raman/Dropbox/b/r/tshirts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C980D32-6E65-9449-B628-186289CF61D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37398CC8-C04A-724B-AFFC-781797AD5847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outgoing" sheetId="1" r:id="rId1"/>
@@ -570,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,6 +896,18 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ECAB8CA3-F73B-CC40-A039-895B30779B4E}">
+          <x14:formula1>
+            <xm:f>incoming!$B$1:$M$1</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1003,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>